<commit_message>
first Commit With Hello World Using Java Configuration Instead of Web xml Configuration
</commit_message>
<xml_diff>
--- a/ANSARI_ZAID_PROJECT_2_ERRORS AND SOLUTIONS.xlsx
+++ b/ANSARI_ZAID_PROJECT_2_ERRORS AND SOLUTIONS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Niit\ZaidEcommerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\zaid_onlineCollaboration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4995"/>
   </bookViews>
   <sheets>
     <sheet name="DAY_01" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>S.No</t>
   </si>
@@ -77,36 +77,6 @@
   <si>
     <t>Reference Site 
 URL</t>
-  </si>
-  <si>
-    <t>INSTALLING TOMCAT SERVER IN ECLIPSE</t>
-  </si>
-  <si>
-    <t>http://www.eclipse.org/webtools/jst/components/ws/1.5/tutorials/InstallTomcat/InstallTomcat.html</t>
-  </si>
-  <si>
-    <t>http://crunchify.com/step-by-step-guide-to-setup-and-install-apache-tomcat-server-in-eclipse-development-environment-ide/</t>
-  </si>
-  <si>
-    <t>10 MIN</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>ADDING MAVEN PROJECT</t>
-  </si>
-  <si>
-    <t>5 MIN</t>
-  </si>
-  <si>
-    <t>CREATING README FILE AND .GITIGNORE</t>
-  </si>
-  <si>
-    <t>1MIN</t>
-  </si>
-  <si>
-    <t>UPLOADING FILE ON GIT</t>
   </si>
 </sst>
 </file>
@@ -542,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,78 +555,38 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
-        <v>42656</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="A2" s="15"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>42656</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="A3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="6"/>
-      <c r="F3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7">
-        <v>42656</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="A4" s="15"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7">
-        <v>42656</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="A5" s="15"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="9"/>
       <c r="E5" s="4"/>
       <c r="F5" s="8"/>
@@ -679,11 +609,8 @@
       <c r="B7" s="14"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>